<commit_message>
added the results tables
</commit_message>
<xml_diff>
--- a/data/lbmbenchmark.xlsx
+++ b/data/lbmbenchmark.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CPU" sheetId="1" r:id="rId1"/>
     <sheet name="GPU" sheetId="2" r:id="rId2"/>
     <sheet name="Chart1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>CPU LBM</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -528,11 +531,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="510056728"/>
-        <c:axId val="509872344"/>
+        <c:axId val="493228504"/>
+        <c:axId val="493235432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="510056728"/>
+        <c:axId val="493228504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="528.0"/>
@@ -562,13 +565,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509872344"/>
+        <c:crossAx val="493235432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="16.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="509872344"/>
+        <c:axId val="493235432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,7 +601,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510056728"/>
+        <c:crossAx val="493228504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -619,7 +622,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="149" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -977,9 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E16:E34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -1007,6 +1008,9 @@
       <c r="D2">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -1042,7 +1046,7 @@
         <v>1.2408710000000001</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E34" si="0">AVERAGE(B4:D4)</f>
+        <f t="shared" ref="E4:E15" si="0">AVERAGE(B4:D4)</f>
         <v>1.2402430000000002</v>
       </c>
     </row>
@@ -2028,7 +2032,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>